<commit_message>
Your descriptive commit message here
</commit_message>
<xml_diff>
--- a/data10th.xlsx
+++ b/data10th.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="147">
   <si>
     <t>SR</t>
   </si>
@@ -153,24 +153,15 @@
     <t>Umang Verma</t>
   </si>
   <si>
-    <t>Roshani</t>
-  </si>
-  <si>
     <t>Tamanna</t>
   </si>
   <si>
-    <t>Janvi</t>
-  </si>
-  <si>
     <t>Aarti</t>
   </si>
   <si>
     <t>Mahima</t>
   </si>
   <si>
-    <t>Khusbhu</t>
-  </si>
-  <si>
     <t>Deepika</t>
   </si>
   <si>
@@ -234,9 +225,6 @@
     <t>Sanjana</t>
   </si>
   <si>
-    <t>Mr. Satywan Verma</t>
-  </si>
-  <si>
     <t>Mr. Banke Bihari</t>
   </si>
   <si>
@@ -258,12 +246,6 @@
     <t>Mr. Balvinder</t>
   </si>
   <si>
-    <t>Mr. Devender</t>
-  </si>
-  <si>
-    <t>Mr. Soni</t>
-  </si>
-  <si>
     <t>Mr. Vijay</t>
   </si>
   <si>
@@ -279,9 +261,6 @@
     <t>Mr. Parmod</t>
   </si>
   <si>
-    <t>Mr. Karam Singh</t>
-  </si>
-  <si>
     <t>Mr. Mangat Ram</t>
   </si>
   <si>
@@ -318,9 +297,6 @@
     <t>Mr. Rinku</t>
   </si>
   <si>
-    <t>Mr. Satish</t>
-  </si>
-  <si>
     <t>HPS10013</t>
   </si>
   <si>
@@ -370,6 +346,117 @@
   </si>
   <si>
     <t>HPS10029</t>
+  </si>
+  <si>
+    <t>10001.jpg</t>
+  </si>
+  <si>
+    <t>10002.jpg</t>
+  </si>
+  <si>
+    <t>10003.jpg</t>
+  </si>
+  <si>
+    <t>10004.jpg</t>
+  </si>
+  <si>
+    <t>10005.jpg</t>
+  </si>
+  <si>
+    <t>10006.jpg</t>
+  </si>
+  <si>
+    <t>10007.jpg</t>
+  </si>
+  <si>
+    <t>10008.jpg</t>
+  </si>
+  <si>
+    <t>10009.jpg</t>
+  </si>
+  <si>
+    <t>10010.jpg</t>
+  </si>
+  <si>
+    <t>10011.jpg</t>
+  </si>
+  <si>
+    <t>10012.jpg</t>
+  </si>
+  <si>
+    <t>10013.jpg</t>
+  </si>
+  <si>
+    <t>10014.jpg</t>
+  </si>
+  <si>
+    <t>10015.jpg</t>
+  </si>
+  <si>
+    <t>10016.jpg</t>
+  </si>
+  <si>
+    <t>10017.jpg</t>
+  </si>
+  <si>
+    <t>10018.jpg</t>
+  </si>
+  <si>
+    <t>10019.jpg</t>
+  </si>
+  <si>
+    <t>10020.jpg</t>
+  </si>
+  <si>
+    <t>10021.jpg</t>
+  </si>
+  <si>
+    <t>10022.jpg</t>
+  </si>
+  <si>
+    <t>10023.jpg</t>
+  </si>
+  <si>
+    <t>10024.jpg</t>
+  </si>
+  <si>
+    <t>10025.jpg</t>
+  </si>
+  <si>
+    <t>10026.jpg</t>
+  </si>
+  <si>
+    <t>10027.jpg</t>
+  </si>
+  <si>
+    <t>10028.jpg</t>
+  </si>
+  <si>
+    <t>10029.jpg</t>
+  </si>
+  <si>
+    <t>Roshni</t>
+  </si>
+  <si>
+    <t>Mr. Satyawan Verma</t>
+  </si>
+  <si>
+    <t>Mr. Davender</t>
+  </si>
+  <si>
+    <t>Mr. Karan Singh</t>
+  </si>
+  <si>
+    <t>Mr. Satish Kumar</t>
+  </si>
+  <si>
+    <t>Tanvi</t>
+  </si>
+  <si>
+    <t>Khushbu</t>
+  </si>
+  <si>
+    <t>Mr. Sonu Soni</t>
   </si>
 </sst>
 </file>
@@ -405,9 +492,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,17 +795,17 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="25.88671875" customWidth="1"/>
-    <col min="6" max="6" width="36.109375" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -735,7 +825,7 @@
       <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G1" t="s">
@@ -762,7 +852,7 @@
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -770,8 +860,8 @@
       <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
-        <v>27</v>
+      <c r="F2" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -794,10 +884,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -805,8 +895,8 @@
       <c r="E3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
-        <v>28</v>
+      <c r="F3" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -829,10 +919,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -840,8 +930,8 @@
       <c r="E4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
-        <v>29</v>
+      <c r="F4" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -864,10 +954,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -875,8 +965,8 @@
       <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="F5" t="s">
-        <v>30</v>
+      <c r="F5" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -899,10 +989,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -910,8 +1000,8 @@
       <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="F6" t="s">
-        <v>31</v>
+      <c r="F6" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
@@ -934,10 +1024,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -945,8 +1035,8 @@
       <c r="E7" t="s">
         <v>37</v>
       </c>
-      <c r="F7" t="s">
-        <v>27</v>
+      <c r="F7" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
@@ -969,10 +1059,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -980,8 +1070,8 @@
       <c r="E8" t="s">
         <v>38</v>
       </c>
-      <c r="F8" t="s">
-        <v>28</v>
+      <c r="F8" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
@@ -1004,10 +1094,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1015,8 +1105,8 @@
       <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="F9" t="s">
-        <v>29</v>
+      <c r="F9" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="G9" t="s">
         <v>15</v>
@@ -1039,10 +1129,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1050,8 +1140,8 @@
       <c r="E10" t="s">
         <v>40</v>
       </c>
-      <c r="F10" t="s">
-        <v>30</v>
+      <c r="F10" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="G10" t="s">
         <v>16</v>
@@ -1074,10 +1164,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -1085,8 +1175,8 @@
       <c r="E11" t="s">
         <v>41</v>
       </c>
-      <c r="F11" t="s">
-        <v>31</v>
+      <c r="F11" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="G11" t="s">
         <v>17</v>
@@ -1109,10 +1199,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -1120,8 +1210,8 @@
       <c r="E12" t="s">
         <v>42</v>
       </c>
-      <c r="F12" t="s">
-        <v>27</v>
+      <c r="F12" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G12" t="s">
         <v>18</v>
@@ -1144,10 +1234,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -1155,8 +1245,8 @@
       <c r="E13" t="s">
         <v>43</v>
       </c>
-      <c r="F13" t="s">
-        <v>28</v>
+      <c r="F13" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
@@ -1179,16 +1269,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>93</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1196,16 +1289,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>94</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="G15" t="s">
         <v>27</v>
@@ -1216,16 +1312,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="G16" t="s">
         <v>28</v>
@@ -1236,16 +1335,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="G17" t="s">
         <v>29</v>
@@ -1256,16 +1358,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>97</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="G18" t="s">
         <v>30</v>
@@ -1276,16 +1381,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>98</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="G19" t="s">
         <v>31</v>
@@ -1296,16 +1404,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>99</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="G20" t="s">
         <v>27</v>
@@ -1316,16 +1427,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>100</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="G21" t="s">
         <v>28</v>
@@ -1336,16 +1450,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
+        <v>101</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="G22" t="s">
         <v>29</v>
@@ -1356,16 +1473,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>110</v>
+        <v>102</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="G23" t="s">
         <v>30</v>
@@ -1376,16 +1496,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>111</v>
+        <v>103</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="G24" t="s">
         <v>31</v>
@@ -1396,16 +1519,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="G25" t="s">
         <v>27</v>
@@ -1416,16 +1542,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>113</v>
+        <v>105</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="G26" t="s">
         <v>28</v>
@@ -1436,16 +1565,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>114</v>
+        <v>106</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1453,16 +1585,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>115</v>
+        <v>107</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1470,16 +1605,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>108</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1487,16 +1625,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>117</v>
+        <v>109</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1510,7 +1651,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1522,7 +1663,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>